<commit_message>
update the problems list
</commit_message>
<xml_diff>
--- a/usaco.xlsx
+++ b/usaco.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project\cpp\usaco_cpp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5403DAC8-B21B-43D2-8E76-E7ECC161E3C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D0D57E0-6CD2-43DF-B697-B87D133DD99A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="293">
   <si>
     <t>难度</t>
   </si>
@@ -1078,6 +1078,80 @@
   </si>
   <si>
     <t>bfs无向图全连接检测</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>单向图</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.usaco.org/index.php?page=viewproblem2&amp;cpid=992</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">
+USACO 2020 January Contest, Silver
+Problem 3. Wormhole Sort</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>二分</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">upper_bound + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>并查集</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.usaco.org/index.php?page=viewproblem2&amp;cpid=1159</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">
+USACO 2021 December Contest, Silver
+Problem 2. Connecting Two Barns</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>连通分量(并查集) + 二分 + 优先级队列</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://usaco.org/index.php?page=viewproblem2&amp;cpid=1206</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">
+USACO 2022 February Contest, Silver
+Problem 1. Redistributing Gifts</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>dfs+reach[i][j] 环检测</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -1085,7 +1159,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1122,6 +1196,26 @@
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1166,7 +1260,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1191,6 +1285,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3017,8 +3114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6204EDAC-36DE-45DA-9D05-C0DF780A7104}">
   <dimension ref="A1:D74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="56.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3026,7 +3123,7 @@
     <col min="1" max="1" width="33.5" style="5" customWidth="1"/>
     <col min="2" max="2" width="24.5" style="6" customWidth="1"/>
     <col min="3" max="3" width="14.83203125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="28.6640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="33.9140625" style="4" customWidth="1"/>
     <col min="5" max="6" width="12.83203125" style="4" customWidth="1"/>
     <col min="7" max="8" width="14.08203125" style="4" customWidth="1"/>
     <col min="9" max="10" width="19.83203125" style="4" customWidth="1"/>
@@ -3496,20 +3593,60 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="6"/>
-      <c r="B34" s="3"/>
+      <c r="A34" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="35" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="6"/>
-      <c r="B35" s="3"/>
+      <c r="A35" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="36" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="6"/>
-      <c r="B36" s="3"/>
+      <c r="A36" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="37" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="6"/>
-      <c r="B37" s="3"/>
+      <c r="A37" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>292</v>
+      </c>
     </row>
     <row r="38" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="6"/>
@@ -3689,8 +3826,12 @@
     <hyperlink ref="B31" r:id="rId25" xr:uid="{BEAD5244-45CB-450D-878E-88704AD119C3}"/>
     <hyperlink ref="B32" r:id="rId26" xr:uid="{C9F3C241-C00B-4E2F-8B35-266C57CE5DB0}"/>
     <hyperlink ref="B33" r:id="rId27" xr:uid="{94FF9DB2-3C4A-4EF7-B9C7-0A5C05CBF5C0}"/>
+    <hyperlink ref="B34" r:id="rId28" xr:uid="{F368253B-A38F-4CA5-906D-89C92C6B284E}"/>
+    <hyperlink ref="B35" r:id="rId29" xr:uid="{4591C6CD-42E3-4130-84E4-A3688C21CA2F}"/>
+    <hyperlink ref="B36" r:id="rId30" xr:uid="{40780C72-4D5B-4A8C-880A-939C8B86A688}"/>
+    <hyperlink ref="B37" r:id="rId31" xr:uid="{D9BDC97D-3688-47AE-B0FA-221E5A448086}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId28"/>
+  <pageSetup orientation="portrait" r:id="rId32"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
flood fill, flood check, 2-step fence
</commit_message>
<xml_diff>
--- a/usaco.xlsx
+++ b/usaco.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project\cpp\usaco_cpp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8FA4CA0-8240-45B7-AE68-BA6AA2C5D319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4269440-D1F9-411F-B2E2-9B84CFECB808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bronze" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="308">
   <si>
     <t>难度</t>
   </si>
@@ -1194,6 +1194,33 @@
   <si>
     <t>二分+bfs检查各点可达性
 （对效率要求很苛刻）</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.usaco.org/index.php?page=viewproblem2&amp;cpid=570</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>USACO 2015 December Contest, Silver
+Problem 1. Switching on the Lights</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>离散flood fill + flood 检查</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.usaco.org/index.php?page=viewproblem2&amp;cpid=596</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">
+USACO 2016 January Contest, Silver
+Problem 3. Build Gates</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>flood fill + 二维数组模拟fence</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -1618,19 +1645,19 @@
       <selection activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="56.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="56.4" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.4140625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="24.4140625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="14.75" style="4" customWidth="1"/>
+    <col min="1" max="1" width="33.44140625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="24.44140625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="14.77734375" style="4" customWidth="1"/>
     <col min="4" max="4" width="18.33203125" style="4" customWidth="1"/>
-    <col min="5" max="6" width="12.75" style="4" customWidth="1"/>
-    <col min="7" max="8" width="14.08203125" style="4" customWidth="1"/>
-    <col min="9" max="10" width="19.75" style="4" customWidth="1"/>
-    <col min="11" max="16384" width="8.9140625" style="4"/>
+    <col min="5" max="6" width="12.77734375" style="4" customWidth="1"/>
+    <col min="7" max="8" width="14.109375" style="4" customWidth="1"/>
+    <col min="9" max="10" width="19.77734375" style="4" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="1" customFormat="1" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" s="1" customFormat="1" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1704,7 +1731,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
@@ -1718,7 +1745,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
@@ -1732,7 +1759,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>109</v>
       </c>
@@ -1749,7 +1776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>8</v>
       </c>
@@ -1766,7 +1793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>12</v>
       </c>
@@ -1783,7 +1810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>14</v>
       </c>
@@ -1800,7 +1827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>21</v>
       </c>
@@ -1814,7 +1841,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>23</v>
       </c>
@@ -1831,7 +1858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>25</v>
       </c>
@@ -1851,7 +1878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>27</v>
       </c>
@@ -1868,7 +1895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>31</v>
       </c>
@@ -1885,7 +1912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>17</v>
       </c>
@@ -1905,7 +1932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>35</v>
       </c>
@@ -1922,7 +1949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>37</v>
       </c>
@@ -1939,7 +1966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>38</v>
       </c>
@@ -1959,7 +1986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>40</v>
       </c>
@@ -1976,7 +2003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>42</v>
       </c>
@@ -1993,7 +2020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>45</v>
       </c>
@@ -2007,7 +2034,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="20" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>46</v>
       </c>
@@ -2024,7 +2051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>50</v>
       </c>
@@ -2041,7 +2068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>52</v>
       </c>
@@ -2058,7 +2085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>55</v>
       </c>
@@ -2084,7 +2111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>58</v>
       </c>
@@ -2107,7 +2134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>61</v>
       </c>
@@ -2127,7 +2154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>62</v>
       </c>
@@ -2144,7 +2171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>64</v>
       </c>
@@ -2164,7 +2191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>66</v>
       </c>
@@ -2184,7 +2211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>68</v>
       </c>
@@ -2204,7 +2231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>71</v>
       </c>
@@ -2221,7 +2248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>73</v>
       </c>
@@ -2244,7 +2271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>75</v>
       </c>
@@ -2267,7 +2294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>77</v>
       </c>
@@ -2290,7 +2317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>79</v>
       </c>
@@ -2307,7 +2334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>81</v>
       </c>
@@ -2327,7 +2354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>84</v>
       </c>
@@ -2347,7 +2374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>86</v>
       </c>
@@ -2367,7 +2394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>88</v>
       </c>
@@ -2387,7 +2414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>90</v>
       </c>
@@ -2401,7 +2428,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="40" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>92</v>
       </c>
@@ -2418,7 +2445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>94</v>
       </c>
@@ -2438,7 +2465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>97</v>
       </c>
@@ -2455,7 +2482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
         <v>99</v>
       </c>
@@ -2472,7 +2499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>102</v>
       </c>
@@ -2492,7 +2519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>104</v>
       </c>
@@ -2515,7 +2542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>107</v>
       </c>
@@ -2535,7 +2562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
         <v>112</v>
       </c>
@@ -2552,7 +2579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
         <v>114</v>
       </c>
@@ -2572,7 +2599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
         <v>116</v>
       </c>
@@ -2592,7 +2619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
         <v>119</v>
       </c>
@@ -2615,7 +2642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
         <v>121</v>
       </c>
@@ -2632,7 +2659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
         <v>124</v>
       </c>
@@ -2649,7 +2676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
         <v>126</v>
       </c>
@@ -2669,7 +2696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
         <v>129</v>
       </c>
@@ -2686,7 +2713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
         <v>131</v>
       </c>
@@ -2706,7 +2733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
         <v>133</v>
       </c>
@@ -2723,7 +2750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
         <v>135</v>
       </c>
@@ -2740,7 +2767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
         <v>137</v>
       </c>
@@ -2757,7 +2784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
         <v>139</v>
       </c>
@@ -2780,7 +2807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
         <v>141</v>
       </c>
@@ -2800,7 +2827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
         <v>143</v>
       </c>
@@ -2817,7 +2844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
         <v>145</v>
       </c>
@@ -2834,7 +2861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
         <v>147</v>
       </c>
@@ -2854,7 +2881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
         <v>149</v>
       </c>
@@ -2874,7 +2901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
         <v>151</v>
       </c>
@@ -2894,7 +2921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
         <v>154</v>
       </c>
@@ -2920,7 +2947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
         <v>156</v>
       </c>
@@ -2946,7 +2973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
         <v>157</v>
       </c>
@@ -2972,7 +2999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
         <v>159</v>
       </c>
@@ -2992,7 +3019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
         <v>161</v>
       </c>
@@ -3015,7 +3042,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="8" t="s">
         <v>163</v>
       </c>
@@ -3032,7 +3059,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="8" t="s">
         <v>165</v>
       </c>
@@ -3052,7 +3079,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="8" t="s">
         <v>168</v>
       </c>
@@ -3156,23 +3183,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6204EDAC-36DE-45DA-9D05-C0DF780A7104}">
   <dimension ref="A1:D74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="56.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="56.4" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.4140625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="24.4140625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="14.75" style="4" customWidth="1"/>
-    <col min="4" max="4" width="35.4140625" style="4" customWidth="1"/>
-    <col min="5" max="6" width="12.75" style="4" customWidth="1"/>
-    <col min="7" max="8" width="14.08203125" style="4" customWidth="1"/>
-    <col min="9" max="10" width="19.75" style="4" customWidth="1"/>
-    <col min="11" max="16384" width="8.9140625" style="4"/>
+    <col min="1" max="1" width="33.44140625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="24.44140625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="14.77734375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="35.44140625" style="4" customWidth="1"/>
+    <col min="5" max="6" width="12.77734375" style="4" customWidth="1"/>
+    <col min="7" max="8" width="14.109375" style="4" customWidth="1"/>
+    <col min="9" max="10" width="19.77734375" style="4" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -3186,7 +3213,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>169</v>
       </c>
@@ -3200,7 +3227,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>171</v>
       </c>
@@ -3214,7 +3241,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>173</v>
       </c>
@@ -3228,7 +3255,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>175</v>
       </c>
@@ -3242,7 +3269,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>177</v>
       </c>
@@ -3256,7 +3283,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>179</v>
       </c>
@@ -3270,7 +3297,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>181</v>
       </c>
@@ -3284,7 +3311,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>183</v>
       </c>
@@ -3298,7 +3325,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>185</v>
       </c>
@@ -3312,7 +3339,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>187</v>
       </c>
@@ -3326,7 +3353,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>189</v>
       </c>
@@ -3340,7 +3367,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>191</v>
       </c>
@@ -3354,7 +3381,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>193</v>
       </c>
@@ -3368,7 +3395,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>195</v>
       </c>
@@ -3382,7 +3409,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>197</v>
       </c>
@@ -3396,7 +3423,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>214</v>
       </c>
@@ -3410,7 +3437,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>218</v>
       </c>
@@ -3424,7 +3451,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>221</v>
       </c>
@@ -3438,7 +3465,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>222</v>
       </c>
@@ -3452,7 +3479,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>225</v>
       </c>
@@ -3466,7 +3493,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>228</v>
       </c>
@@ -3480,7 +3507,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>231</v>
       </c>
@@ -3494,7 +3521,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>234</v>
       </c>
@@ -3508,7 +3535,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>237</v>
       </c>
@@ -3522,7 +3549,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>240</v>
       </c>
@@ -3536,7 +3563,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>243</v>
       </c>
@@ -3550,7 +3577,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>246</v>
       </c>
@@ -3564,7 +3591,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>248</v>
       </c>
@@ -3578,7 +3605,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>251</v>
       </c>
@@ -3592,7 +3619,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>254</v>
       </c>
@@ -3606,7 +3633,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>278</v>
       </c>
@@ -3620,7 +3647,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>281</v>
       </c>
@@ -3634,7 +3661,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>278</v>
       </c>
@@ -3648,7 +3675,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>285</v>
       </c>
@@ -3662,7 +3689,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>288</v>
       </c>
@@ -3676,7 +3703,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>291</v>
       </c>
@@ -3690,7 +3717,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>294</v>
       </c>
@@ -3704,7 +3731,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>297</v>
       </c>
@@ -3718,7 +3745,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>300</v>
       </c>
@@ -3732,139 +3759,159 @@
         <v>301</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="6"/>
-      <c r="B41" s="3"/>
-    </row>
-    <row r="42" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="6"/>
-      <c r="B42" s="3"/>
-    </row>
-    <row r="43" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="6"/>
       <c r="B43" s="3"/>
     </row>
-    <row r="44" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="6"/>
       <c r="B44" s="3"/>
     </row>
-    <row r="45" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="6"/>
       <c r="B45" s="3"/>
     </row>
-    <row r="46" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="6"/>
       <c r="B46" s="3"/>
     </row>
-    <row r="47" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="6"/>
       <c r="B47" s="3"/>
     </row>
-    <row r="48" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="6"/>
       <c r="B48" s="3"/>
     </row>
-    <row r="49" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="6"/>
       <c r="B49" s="3"/>
     </row>
-    <row r="50" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="6"/>
       <c r="B50" s="3"/>
     </row>
-    <row r="51" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="6"/>
       <c r="B51" s="3"/>
     </row>
-    <row r="52" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="6"/>
       <c r="B52" s="3"/>
     </row>
-    <row r="53" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="6"/>
       <c r="B53" s="3"/>
     </row>
-    <row r="54" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="6"/>
       <c r="B54" s="3"/>
     </row>
-    <row r="55" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="6"/>
       <c r="B55" s="3"/>
     </row>
-    <row r="56" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="6"/>
       <c r="B56" s="3"/>
     </row>
-    <row r="57" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="6"/>
       <c r="B57" s="3"/>
     </row>
-    <row r="58" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="6"/>
       <c r="B58" s="3"/>
     </row>
-    <row r="59" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="6"/>
       <c r="B59" s="3"/>
     </row>
-    <row r="60" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="6"/>
       <c r="B60" s="3"/>
     </row>
-    <row r="61" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="6"/>
       <c r="B61" s="3"/>
     </row>
-    <row r="62" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="6"/>
       <c r="B62" s="3"/>
     </row>
-    <row r="63" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="6"/>
       <c r="B63" s="3"/>
     </row>
-    <row r="64" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="6"/>
       <c r="B64" s="3"/>
     </row>
-    <row r="65" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="6"/>
       <c r="B65" s="3"/>
     </row>
-    <row r="66" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="6"/>
       <c r="B66" s="3"/>
     </row>
-    <row r="67" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="6"/>
       <c r="B67" s="3"/>
     </row>
-    <row r="68" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="6"/>
       <c r="B68" s="3"/>
     </row>
-    <row r="69" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="6"/>
       <c r="B69" s="3"/>
     </row>
-    <row r="70" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="6"/>
       <c r="B70" s="3"/>
     </row>
-    <row r="71" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="6"/>
       <c r="B71" s="3"/>
     </row>
-    <row r="72" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="8"/>
       <c r="B72" s="3"/>
     </row>
-    <row r="73" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="8"/>
       <c r="B73" s="3"/>
     </row>
-    <row r="74" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="8"/>
       <c r="B74" s="3"/>
     </row>
@@ -3905,8 +3952,10 @@
     <hyperlink ref="B38" r:id="rId32" xr:uid="{B475B256-967C-4F64-A4DD-526CEDC26042}"/>
     <hyperlink ref="B39" r:id="rId33" xr:uid="{779F75BC-4D59-437A-9D4D-B9A710F5CA4F}"/>
     <hyperlink ref="B40" r:id="rId34" xr:uid="{8EF40E9D-AAD0-49BA-ABB4-D948C6264B77}"/>
+    <hyperlink ref="B41" r:id="rId35" xr:uid="{072B07CF-9957-46DE-9CDE-3BA1DF0494C5}"/>
+    <hyperlink ref="B42" r:id="rId36" xr:uid="{94A572EA-DCFE-4DBE-BE38-367F3F128FDA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId35"/>
+  <pageSetup orientation="portrait" r:id="rId37"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
flood fill counting + flood fill changing + 双指针更新棋盘状态
</commit_message>
<xml_diff>
--- a/usaco.xlsx
+++ b/usaco.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project\cpp\usaco_cpp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3C4A832-A7D1-495A-8150-FBF7AA1D8EED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8929E866-9DDE-480B-AB59-80DFD5FBE8CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bronze" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="322">
   <si>
     <t>难度</t>
   </si>
@@ -1260,6 +1260,28 @@
   </si>
   <si>
     <t>逆向 flood fill</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.usaco.org/index.php?page=viewproblem2&amp;cpid=860</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>USACO 2018 December Contest, Silver
+Problem 3. Mooyo Mooyo</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>flood fill counting + flood fill changing
++ 双指针更新棋盘状态</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>备注</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>泡泡龙游戏</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -1684,19 +1706,19 @@
       <selection activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="56.4" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="56.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.44140625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="24.44140625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="14.77734375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="33.4140625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="24.4140625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="14.75" style="4" customWidth="1"/>
     <col min="4" max="4" width="18.33203125" style="4" customWidth="1"/>
-    <col min="5" max="6" width="12.77734375" style="4" customWidth="1"/>
-    <col min="7" max="8" width="14.109375" style="4" customWidth="1"/>
-    <col min="9" max="10" width="19.77734375" style="4" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="4"/>
+    <col min="5" max="6" width="12.75" style="4" customWidth="1"/>
+    <col min="7" max="8" width="14.08203125" style="4" customWidth="1"/>
+    <col min="9" max="10" width="19.75" style="4" customWidth="1"/>
+    <col min="11" max="16384" width="8.9140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="1" customFormat="1" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" s="1" customFormat="1" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1770,7 +1792,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
@@ -1784,7 +1806,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
@@ -1798,7 +1820,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>109</v>
       </c>
@@ -1815,7 +1837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>8</v>
       </c>
@@ -1832,7 +1854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>12</v>
       </c>
@@ -1849,7 +1871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>14</v>
       </c>
@@ -1866,7 +1888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>21</v>
       </c>
@@ -1880,7 +1902,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>23</v>
       </c>
@@ -1897,7 +1919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>25</v>
       </c>
@@ -1917,7 +1939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>27</v>
       </c>
@@ -1934,7 +1956,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>31</v>
       </c>
@@ -1951,7 +1973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>17</v>
       </c>
@@ -1971,7 +1993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>35</v>
       </c>
@@ -1988,7 +2010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>37</v>
       </c>
@@ -2005,7 +2027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>38</v>
       </c>
@@ -2025,7 +2047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>40</v>
       </c>
@@ -2042,7 +2064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>42</v>
       </c>
@@ -2059,7 +2081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>45</v>
       </c>
@@ -2073,7 +2095,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="20" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>46</v>
       </c>
@@ -2090,7 +2112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>50</v>
       </c>
@@ -2107,7 +2129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>52</v>
       </c>
@@ -2124,7 +2146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>55</v>
       </c>
@@ -2150,7 +2172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>58</v>
       </c>
@@ -2173,7 +2195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>61</v>
       </c>
@@ -2193,7 +2215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>62</v>
       </c>
@@ -2210,7 +2232,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
         <v>64</v>
       </c>
@@ -2230,7 +2252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
         <v>66</v>
       </c>
@@ -2250,7 +2272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
         <v>68</v>
       </c>
@@ -2270,7 +2292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
         <v>71</v>
       </c>
@@ -2287,7 +2309,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
         <v>73</v>
       </c>
@@ -2310,7 +2332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>75</v>
       </c>
@@ -2333,7 +2355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
         <v>77</v>
       </c>
@@ -2356,7 +2378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
         <v>79</v>
       </c>
@@ -2373,7 +2395,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
         <v>81</v>
       </c>
@@ -2393,7 +2415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
         <v>84</v>
       </c>
@@ -2413,7 +2435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
         <v>86</v>
       </c>
@@ -2433,7 +2455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="6" t="s">
         <v>88</v>
       </c>
@@ -2453,7 +2475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
         <v>90</v>
       </c>
@@ -2467,7 +2489,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="40" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="6" t="s">
         <v>92</v>
       </c>
@@ -2484,7 +2506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
         <v>94</v>
       </c>
@@ -2504,7 +2526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="6" t="s">
         <v>97</v>
       </c>
@@ -2521,7 +2543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="6" t="s">
         <v>99</v>
       </c>
@@ -2538,7 +2560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="6" t="s">
         <v>102</v>
       </c>
@@ -2558,7 +2580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="6" t="s">
         <v>104</v>
       </c>
@@ -2581,7 +2603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="6" t="s">
         <v>107</v>
       </c>
@@ -2601,7 +2623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="6" t="s">
         <v>112</v>
       </c>
@@ -2618,7 +2640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="6" t="s">
         <v>114</v>
       </c>
@@ -2638,7 +2660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="6" t="s">
         <v>116</v>
       </c>
@@ -2658,7 +2680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
         <v>119</v>
       </c>
@@ -2681,7 +2703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="6" t="s">
         <v>121</v>
       </c>
@@ -2698,7 +2720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="6" t="s">
         <v>124</v>
       </c>
@@ -2715,7 +2737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="6" t="s">
         <v>126</v>
       </c>
@@ -2735,7 +2757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="6" t="s">
         <v>129</v>
       </c>
@@ -2752,7 +2774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="6" t="s">
         <v>131</v>
       </c>
@@ -2772,7 +2794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="6" t="s">
         <v>133</v>
       </c>
@@ -2789,7 +2811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="6" t="s">
         <v>135</v>
       </c>
@@ -2806,7 +2828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="6" t="s">
         <v>137</v>
       </c>
@@ -2823,7 +2845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="6" t="s">
         <v>139</v>
       </c>
@@ -2846,7 +2868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="6" t="s">
         <v>141</v>
       </c>
@@ -2866,7 +2888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="6" t="s">
         <v>143</v>
       </c>
@@ -2883,7 +2905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="6" t="s">
         <v>145</v>
       </c>
@@ -2900,7 +2922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="6" t="s">
         <v>147</v>
       </c>
@@ -2920,7 +2942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="6" t="s">
         <v>149</v>
       </c>
@@ -2940,7 +2962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="6" t="s">
         <v>151</v>
       </c>
@@ -2960,7 +2982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="6" t="s">
         <v>154</v>
       </c>
@@ -2986,7 +3008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="6" t="s">
         <v>156</v>
       </c>
@@ -3012,7 +3034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="6" t="s">
         <v>157</v>
       </c>
@@ -3038,7 +3060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="6" t="s">
         <v>159</v>
       </c>
@@ -3058,7 +3080,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="6" t="s">
         <v>161</v>
       </c>
@@ -3081,7 +3103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="8" t="s">
         <v>163</v>
       </c>
@@ -3098,7 +3120,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="8" t="s">
         <v>165</v>
       </c>
@@ -3118,7 +3140,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="8" t="s">
         <v>168</v>
       </c>
@@ -3220,25 +3242,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6204EDAC-36DE-45DA-9D05-C0DF780A7104}">
-  <dimension ref="A1:D74"/>
+  <dimension ref="A1:E74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="56.4" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="56.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.44140625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="24.44140625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="14.77734375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="35.44140625" style="4" customWidth="1"/>
-    <col min="5" max="6" width="12.77734375" style="4" customWidth="1"/>
-    <col min="7" max="8" width="14.109375" style="4" customWidth="1"/>
-    <col min="9" max="10" width="19.77734375" style="4" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="4"/>
+    <col min="1" max="1" width="33.4140625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="24.4140625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="14.75" style="4" customWidth="1"/>
+    <col min="4" max="4" width="35.4140625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="22.1640625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="12.75" style="4" customWidth="1"/>
+    <col min="7" max="8" width="14.08203125" style="4" customWidth="1"/>
+    <col min="9" max="10" width="19.75" style="4" customWidth="1"/>
+    <col min="11" max="16384" width="8.9140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -3251,8 +3274,11 @@
       <c r="D1" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>169</v>
       </c>
@@ -3266,7 +3292,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>171</v>
       </c>
@@ -3280,7 +3306,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>173</v>
       </c>
@@ -3294,7 +3320,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>175</v>
       </c>
@@ -3308,7 +3334,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>177</v>
       </c>
@@ -3322,7 +3348,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>179</v>
       </c>
@@ -3336,7 +3362,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>181</v>
       </c>
@@ -3350,7 +3376,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>183</v>
       </c>
@@ -3364,7 +3390,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>185</v>
       </c>
@@ -3378,7 +3404,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>187</v>
       </c>
@@ -3392,7 +3418,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>189</v>
       </c>
@@ -3406,7 +3432,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>191</v>
       </c>
@@ -3420,7 +3446,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>193</v>
       </c>
@@ -3434,7 +3460,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>195</v>
       </c>
@@ -3448,7 +3474,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>197</v>
       </c>
@@ -3462,7 +3488,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>214</v>
       </c>
@@ -3476,7 +3502,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>218</v>
       </c>
@@ -3490,7 +3516,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>221</v>
       </c>
@@ -3504,7 +3530,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>222</v>
       </c>
@@ -3518,7 +3544,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>225</v>
       </c>
@@ -3532,7 +3558,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>228</v>
       </c>
@@ -3546,7 +3572,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>231</v>
       </c>
@@ -3560,7 +3586,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>234</v>
       </c>
@@ -3574,7 +3600,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>237</v>
       </c>
@@ -3588,7 +3614,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>240</v>
       </c>
@@ -3602,7 +3628,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
         <v>243</v>
       </c>
@@ -3616,7 +3642,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
         <v>246</v>
       </c>
@@ -3630,7 +3656,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
         <v>248</v>
       </c>
@@ -3644,7 +3670,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
         <v>251</v>
       </c>
@@ -3658,7 +3684,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
         <v>254</v>
       </c>
@@ -3672,7 +3698,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>278</v>
       </c>
@@ -3686,7 +3712,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
         <v>281</v>
       </c>
@@ -3700,7 +3726,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
         <v>278</v>
       </c>
@@ -3714,7 +3740,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
         <v>285</v>
       </c>
@@ -3728,7 +3754,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
         <v>288</v>
       </c>
@@ -3742,7 +3768,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
         <v>291</v>
       </c>
@@ -3756,7 +3782,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="6" t="s">
         <v>294</v>
       </c>
@@ -3770,7 +3796,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
         <v>297</v>
       </c>
@@ -3784,7 +3810,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="6" t="s">
         <v>300</v>
       </c>
@@ -3798,7 +3824,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
         <v>303</v>
       </c>
@@ -3812,7 +3838,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="6" t="s">
         <v>306</v>
       </c>
@@ -3826,7 +3852,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="6" t="s">
         <v>309</v>
       </c>
@@ -3840,7 +3866,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="6" t="s">
         <v>312</v>
       </c>
@@ -3854,7 +3880,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="6" t="s">
         <v>315</v>
       </c>
@@ -3868,119 +3894,132 @@
         <v>316</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="6"/>
-      <c r="B46" s="3"/>
-    </row>
-    <row r="47" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="6"/>
       <c r="B47" s="3"/>
     </row>
-    <row r="48" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="6"/>
       <c r="B48" s="3"/>
     </row>
-    <row r="49" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="6"/>
       <c r="B49" s="3"/>
     </row>
-    <row r="50" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="6"/>
       <c r="B50" s="3"/>
     </row>
-    <row r="51" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="6"/>
       <c r="B51" s="3"/>
     </row>
-    <row r="52" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="6"/>
       <c r="B52" s="3"/>
     </row>
-    <row r="53" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="6"/>
       <c r="B53" s="3"/>
     </row>
-    <row r="54" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="6"/>
       <c r="B54" s="3"/>
     </row>
-    <row r="55" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="6"/>
       <c r="B55" s="3"/>
     </row>
-    <row r="56" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="6"/>
       <c r="B56" s="3"/>
     </row>
-    <row r="57" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="6"/>
       <c r="B57" s="3"/>
     </row>
-    <row r="58" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="6"/>
       <c r="B58" s="3"/>
     </row>
-    <row r="59" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="6"/>
       <c r="B59" s="3"/>
     </row>
-    <row r="60" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="6"/>
       <c r="B60" s="3"/>
     </row>
-    <row r="61" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="6"/>
       <c r="B61" s="3"/>
     </row>
-    <row r="62" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="6"/>
       <c r="B62" s="3"/>
     </row>
-    <row r="63" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="6"/>
       <c r="B63" s="3"/>
     </row>
-    <row r="64" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="6"/>
       <c r="B64" s="3"/>
     </row>
-    <row r="65" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="6"/>
       <c r="B65" s="3"/>
     </row>
-    <row r="66" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="6"/>
       <c r="B66" s="3"/>
     </row>
-    <row r="67" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="6"/>
       <c r="B67" s="3"/>
     </row>
-    <row r="68" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="6"/>
       <c r="B68" s="3"/>
     </row>
-    <row r="69" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="6"/>
       <c r="B69" s="3"/>
     </row>
-    <row r="70" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="6"/>
       <c r="B70" s="3"/>
     </row>
-    <row r="71" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="6"/>
       <c r="B71" s="3"/>
     </row>
-    <row r="72" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="8"/>
       <c r="B72" s="3"/>
     </row>
-    <row r="73" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="8"/>
       <c r="B73" s="3"/>
     </row>
-    <row r="74" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="8"/>
       <c r="B74" s="3"/>
     </row>
@@ -4026,8 +4065,9 @@
     <hyperlink ref="B43" r:id="rId37" xr:uid="{ADBF7BDF-CA54-48E4-B4F9-6D62775BE4C5}"/>
     <hyperlink ref="B44" r:id="rId38" xr:uid="{DBCA6D58-459A-4A9A-BA5E-0A30B08949C0}"/>
     <hyperlink ref="B45" r:id="rId39" xr:uid="{0E912A48-8312-472F-AD5E-A49D20AA7ABB}"/>
+    <hyperlink ref="B46" r:id="rId40" xr:uid="{B7275F49-7890-4FFB-B9AE-74CBC23E91BC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId40"/>
+  <pageSetup orientation="portrait" r:id="rId41"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
C(40,20)优化 + pair hash
</commit_message>
<xml_diff>
--- a/usaco.xlsx
+++ b/usaco.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project\cpp\usaco_cpp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1581AE8-B922-4EE2-8ACB-076251E1B722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4782E611-A00D-4797-A282-15BE632AC422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="338">
   <si>
     <t>难度</t>
   </si>
@@ -1340,6 +1340,19 @@
   </si>
   <si>
     <t>stack +贪心</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.usaco.org/index.php?page=viewproblem2&amp;cpid=1207</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>USACO 2022 February Contest, Silver
+Problem 2. Robot Instructions</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>C(40,20) 的优化 + pair hash</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -3305,8 +3318,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6204EDAC-36DE-45DA-9D05-C0DF780A7104}">
   <dimension ref="A1:E74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="56.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4032,8 +4045,18 @@
       </c>
     </row>
     <row r="51" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="6"/>
-      <c r="B51" s="3"/>
+      <c r="A51" s="6" t="s">
+        <v>336</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>337</v>
+      </c>
     </row>
     <row r="52" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="6"/>
@@ -4173,8 +4196,9 @@
     <hyperlink ref="B47" r:id="rId41" xr:uid="{BA57EB9A-AF36-4E7D-8B9D-8DB57DBD486D}"/>
     <hyperlink ref="B48" r:id="rId42" xr:uid="{2B53B0AC-35AD-48FC-8E94-6EDC4E4E0E16}"/>
     <hyperlink ref="B49" r:id="rId43" xr:uid="{08DC754E-03B2-4643-9F3F-110315B91B01}"/>
+    <hyperlink ref="B51" r:id="rId44" xr:uid="{4ABE615F-540A-476D-AF7C-515849DDC539}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId44"/>
+  <pageSetup orientation="portrait" r:id="rId45"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
hash 离散化 2D-grid + dfs
</commit_message>
<xml_diff>
--- a/usaco.xlsx
+++ b/usaco.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project\cpp\usaco_cpp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A00E1B5D-E226-40A7-8BB1-35E6D3E14540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87B5E058-09DC-4F3D-84FA-DD3CEA4B1DD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bronze" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="350">
   <si>
     <t>难度</t>
   </si>
@@ -1392,6 +1392,19 @@
   </si>
   <si>
     <t>单调栈</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.usaco.org/index.php?page=viewproblem2&amp;cpid=1110</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>USACO 2021 February Contest, Silver
+Problem 1. Comfortable Cows</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>hash离散化2D-grid + dfs</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -1819,19 +1832,19 @@
       <selection activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="56.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="56.4" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.4140625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="24.4140625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="14.75" style="4" customWidth="1"/>
+    <col min="1" max="1" width="33.44140625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="24.44140625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="14.77734375" style="4" customWidth="1"/>
     <col min="4" max="4" width="18.33203125" style="4" customWidth="1"/>
-    <col min="5" max="6" width="12.75" style="4" customWidth="1"/>
-    <col min="7" max="8" width="14.08203125" style="4" customWidth="1"/>
-    <col min="9" max="10" width="19.75" style="4" customWidth="1"/>
-    <col min="11" max="16384" width="8.9140625" style="4"/>
+    <col min="5" max="6" width="12.77734375" style="4" customWidth="1"/>
+    <col min="7" max="8" width="14.109375" style="4" customWidth="1"/>
+    <col min="9" max="10" width="19.77734375" style="4" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="1" customFormat="1" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" s="1" customFormat="1" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1905,7 +1918,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
@@ -1919,7 +1932,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
@@ -1933,7 +1946,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>109</v>
       </c>
@@ -1950,7 +1963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>8</v>
       </c>
@@ -1967,7 +1980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>12</v>
       </c>
@@ -1984,7 +1997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>14</v>
       </c>
@@ -2001,7 +2014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>21</v>
       </c>
@@ -2015,7 +2028,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>23</v>
       </c>
@@ -2032,7 +2045,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>25</v>
       </c>
@@ -2052,7 +2065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>27</v>
       </c>
@@ -2069,7 +2082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>31</v>
       </c>
@@ -2086,7 +2099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>17</v>
       </c>
@@ -2106,7 +2119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>35</v>
       </c>
@@ -2123,7 +2136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>37</v>
       </c>
@@ -2140,7 +2153,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>38</v>
       </c>
@@ -2160,7 +2173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>40</v>
       </c>
@@ -2177,7 +2190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>42</v>
       </c>
@@ -2194,7 +2207,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>45</v>
       </c>
@@ -2208,7 +2221,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="20" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>46</v>
       </c>
@@ -2225,7 +2238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>50</v>
       </c>
@@ -2242,7 +2255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>52</v>
       </c>
@@ -2259,7 +2272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>55</v>
       </c>
@@ -2285,7 +2298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>58</v>
       </c>
@@ -2308,7 +2321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>61</v>
       </c>
@@ -2328,7 +2341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>62</v>
       </c>
@@ -2345,7 +2358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>64</v>
       </c>
@@ -2365,7 +2378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>66</v>
       </c>
@@ -2385,7 +2398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>68</v>
       </c>
@@ -2405,7 +2418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>71</v>
       </c>
@@ -2422,7 +2435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>73</v>
       </c>
@@ -2445,7 +2458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>75</v>
       </c>
@@ -2468,7 +2481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>77</v>
       </c>
@@ -2491,7 +2504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>79</v>
       </c>
@@ -2508,7 +2521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>81</v>
       </c>
@@ -2528,7 +2541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>84</v>
       </c>
@@ -2548,7 +2561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>86</v>
       </c>
@@ -2568,7 +2581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>88</v>
       </c>
@@ -2588,7 +2601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>90</v>
       </c>
@@ -2602,7 +2615,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="40" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>92</v>
       </c>
@@ -2619,7 +2632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>94</v>
       </c>
@@ -2639,7 +2652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>97</v>
       </c>
@@ -2656,7 +2669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
         <v>99</v>
       </c>
@@ -2673,7 +2686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>102</v>
       </c>
@@ -2693,7 +2706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>104</v>
       </c>
@@ -2716,7 +2729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>107</v>
       </c>
@@ -2736,7 +2749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
         <v>112</v>
       </c>
@@ -2753,7 +2766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:24" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
         <v>114</v>
       </c>
@@ -2773,7 +2786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
         <v>116</v>
       </c>
@@ -2793,7 +2806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
         <v>119</v>
       </c>
@@ -2816,7 +2829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
         <v>121</v>
       </c>
@@ -2833,7 +2846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
         <v>124</v>
       </c>
@@ -2850,7 +2863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
         <v>126</v>
       </c>
@@ -2870,7 +2883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
         <v>129</v>
       </c>
@@ -2887,7 +2900,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
         <v>131</v>
       </c>
@@ -2907,7 +2920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
         <v>133</v>
       </c>
@@ -2924,7 +2937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
         <v>135</v>
       </c>
@@ -2941,7 +2954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
         <v>137</v>
       </c>
@@ -2958,7 +2971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
         <v>139</v>
       </c>
@@ -2981,7 +2994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
         <v>141</v>
       </c>
@@ -3001,7 +3014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
         <v>143</v>
       </c>
@@ -3018,7 +3031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
         <v>145</v>
       </c>
@@ -3035,7 +3048,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
         <v>147</v>
       </c>
@@ -3055,7 +3068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:19" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
         <v>149</v>
       </c>
@@ -3075,7 +3088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
         <v>151</v>
       </c>
@@ -3095,7 +3108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
         <v>154</v>
       </c>
@@ -3121,7 +3134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
         <v>156</v>
       </c>
@@ -3147,7 +3160,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
         <v>157</v>
       </c>
@@ -3173,7 +3186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
         <v>159</v>
       </c>
@@ -3193,7 +3206,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
         <v>161</v>
       </c>
@@ -3216,7 +3229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="8" t="s">
         <v>163</v>
       </c>
@@ -3233,7 +3246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="8" t="s">
         <v>165</v>
       </c>
@@ -3253,7 +3266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:26" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="8" t="s">
         <v>168</v>
       </c>
@@ -3357,24 +3370,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6204EDAC-36DE-45DA-9D05-C0DF780A7104}">
   <dimension ref="A1:E74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="56.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="56.4" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.4140625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="24.4140625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="14.75" style="4" customWidth="1"/>
-    <col min="4" max="4" width="35.4140625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="22.08203125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="12.75" style="4" customWidth="1"/>
-    <col min="7" max="8" width="14.08203125" style="4" customWidth="1"/>
-    <col min="9" max="10" width="19.75" style="4" customWidth="1"/>
-    <col min="11" max="16384" width="8.9140625" style="4"/>
+    <col min="1" max="1" width="33.44140625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="24.44140625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="14.77734375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="35.44140625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="22.109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="12.77734375" style="4" customWidth="1"/>
+    <col min="7" max="8" width="14.109375" style="4" customWidth="1"/>
+    <col min="9" max="10" width="19.77734375" style="4" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -3391,7 +3404,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>169</v>
       </c>
@@ -3405,7 +3418,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>171</v>
       </c>
@@ -3419,7 +3432,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>173</v>
       </c>
@@ -3433,7 +3446,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>175</v>
       </c>
@@ -3447,7 +3460,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>177</v>
       </c>
@@ -3461,7 +3474,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>179</v>
       </c>
@@ -3475,7 +3488,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>181</v>
       </c>
@@ -3489,7 +3502,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>183</v>
       </c>
@@ -3503,7 +3516,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>185</v>
       </c>
@@ -3517,7 +3530,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>187</v>
       </c>
@@ -3531,7 +3544,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>189</v>
       </c>
@@ -3545,7 +3558,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>191</v>
       </c>
@@ -3559,7 +3572,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>193</v>
       </c>
@@ -3573,7 +3586,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>195</v>
       </c>
@@ -3587,7 +3600,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>197</v>
       </c>
@@ -3601,7 +3614,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>214</v>
       </c>
@@ -3615,7 +3628,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>218</v>
       </c>
@@ -3629,7 +3642,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>221</v>
       </c>
@@ -3643,7 +3656,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>222</v>
       </c>
@@ -3657,7 +3670,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>225</v>
       </c>
@@ -3671,7 +3684,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>228</v>
       </c>
@@ -3685,7 +3698,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>231</v>
       </c>
@@ -3699,7 +3712,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>234</v>
       </c>
@@ -3713,7 +3726,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>237</v>
       </c>
@@ -3727,7 +3740,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>240</v>
       </c>
@@ -3741,7 +3754,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>243</v>
       </c>
@@ -3755,7 +3768,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>246</v>
       </c>
@@ -3769,7 +3782,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>248</v>
       </c>
@@ -3783,7 +3796,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>251</v>
       </c>
@@ -3797,7 +3810,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>254</v>
       </c>
@@ -3811,7 +3824,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>278</v>
       </c>
@@ -3825,7 +3838,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>281</v>
       </c>
@@ -3839,7 +3852,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>278</v>
       </c>
@@ -3853,7 +3866,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>285</v>
       </c>
@@ -3867,7 +3880,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>288</v>
       </c>
@@ -3881,7 +3894,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>291</v>
       </c>
@@ -3895,7 +3908,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>294</v>
       </c>
@@ -3909,7 +3922,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>297</v>
       </c>
@@ -3923,7 +3936,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>300</v>
       </c>
@@ -3937,7 +3950,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>303</v>
       </c>
@@ -3951,7 +3964,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>306</v>
       </c>
@@ -3965,7 +3978,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
         <v>309</v>
       </c>
@@ -3979,7 +3992,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>312</v>
       </c>
@@ -3993,7 +4006,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>315</v>
       </c>
@@ -4007,7 +4020,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>318</v>
       </c>
@@ -4024,7 +4037,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
         <v>323</v>
       </c>
@@ -4038,7 +4051,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
         <v>326</v>
       </c>
@@ -4052,7 +4065,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
         <v>330</v>
       </c>
@@ -4069,7 +4082,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
         <v>333</v>
       </c>
@@ -4083,7 +4096,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
         <v>336</v>
       </c>
@@ -4097,7 +4110,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
         <v>338</v>
       </c>
@@ -4111,7 +4124,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
         <v>342</v>
       </c>
@@ -4125,7 +4138,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
         <v>345</v>
       </c>
@@ -4139,83 +4152,93 @@
         <v>346</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="6"/>
-      <c r="B55" s="3"/>
-    </row>
-    <row r="56" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="6" t="s">
+        <v>348</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="6"/>
       <c r="B56" s="3"/>
     </row>
-    <row r="57" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="6"/>
       <c r="B57" s="3"/>
     </row>
-    <row r="58" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="6"/>
       <c r="B58" s="3"/>
     </row>
-    <row r="59" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="6"/>
       <c r="B59" s="3"/>
     </row>
-    <row r="60" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="6"/>
       <c r="B60" s="3"/>
     </row>
-    <row r="61" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="6"/>
       <c r="B61" s="3"/>
     </row>
-    <row r="62" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="6"/>
       <c r="B62" s="3"/>
     </row>
-    <row r="63" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="6"/>
       <c r="B63" s="3"/>
     </row>
-    <row r="64" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="6"/>
       <c r="B64" s="3"/>
     </row>
-    <row r="65" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="6"/>
       <c r="B65" s="3"/>
     </row>
-    <row r="66" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="6"/>
       <c r="B66" s="3"/>
     </row>
-    <row r="67" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="6"/>
       <c r="B67" s="3"/>
     </row>
-    <row r="68" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="6"/>
       <c r="B68" s="3"/>
     </row>
-    <row r="69" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="6"/>
       <c r="B69" s="3"/>
     </row>
-    <row r="70" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="6"/>
       <c r="B70" s="3"/>
     </row>
-    <row r="71" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="6"/>
       <c r="B71" s="3"/>
     </row>
-    <row r="72" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="8"/>
       <c r="B72" s="3"/>
     </row>
-    <row r="73" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="8"/>
       <c r="B73" s="3"/>
     </row>
-    <row r="74" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" ht="56.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="8"/>
       <c r="B74" s="3"/>
     </row>
@@ -4269,8 +4292,9 @@
     <hyperlink ref="B52" r:id="rId45" xr:uid="{DF93BDDA-2465-4ABF-AF18-0AED25BE4799}"/>
     <hyperlink ref="B53" r:id="rId46" xr:uid="{E633B21E-D277-4AC3-9FBA-A9550AB5D115}"/>
     <hyperlink ref="B54" r:id="rId47" xr:uid="{57A62B80-76A3-4FAB-8074-5138A4BCA73E}"/>
+    <hyperlink ref="B55" r:id="rId48" xr:uid="{63B96D2C-5CB3-4D58-9B99-E002550B0625}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId48"/>
+  <pageSetup orientation="portrait" r:id="rId49"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
multi path + dfs
</commit_message>
<xml_diff>
--- a/usaco.xlsx
+++ b/usaco.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project\cpp\usaco_cpp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1738B2AB-4680-44BB-9D60-08C28D83FE85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA05234-5DC6-49B3-BB60-03F2B1767920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1820" yWindow="1820" windowWidth="19200" windowHeight="10060" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bronze" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="373">
   <si>
     <t>难度</t>
   </si>
@@ -1493,6 +1493,19 @@
   </si>
   <si>
     <t>greedy + prefix + compression</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://usaco.org/index.php?page=viewproblem2&amp;cpid=1304</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>USACO 2023 February Contest, Silver
+Problem 3. Moo Route II</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>build the graph + dfs</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -3456,7 +3469,7 @@
   <dimension ref="A1:E73"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D63" sqref="D63"/>
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="56.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4347,8 +4360,18 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="6"/>
-      <c r="B63" s="3"/>
+      <c r="A63" s="6" t="s">
+        <v>371</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>372</v>
+      </c>
     </row>
     <row r="64" spans="1:4" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="6"/>
@@ -4448,8 +4471,9 @@
     <hyperlink ref="B60" r:id="rId53" xr:uid="{94878CAB-364C-47F1-ACCC-1432DAF028F9}"/>
     <hyperlink ref="B61" r:id="rId54" xr:uid="{0EDD01E7-62E5-4EC4-8DC1-C2F5F2087AD4}"/>
     <hyperlink ref="B62" r:id="rId55" xr:uid="{B527559E-2DE9-487E-81A2-C207D1C6215E}"/>
+    <hyperlink ref="B63" r:id="rId56" xr:uid="{EE48A03E-9E16-402C-A71D-7BABCD0997E0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId56"/>
+  <pageSetup orientation="portrait" r:id="rId57"/>
 </worksheet>
 </file>
</xml_diff>